<commit_message>
Removed google connectivity for all buttons
</commit_message>
<xml_diff>
--- a/Deposit_Records.xlsx
+++ b/Deposit_Records.xlsx
@@ -548,7 +548,7 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>11/08/2020</t>
+          <t>08/11/2020</t>
         </is>
       </c>
     </row>
@@ -610,7 +610,7 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>11/08/2020</t>
+          <t>08/11/2020</t>
         </is>
       </c>
     </row>
@@ -734,7 +734,7 @@
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>10/06/2020</t>
+          <t>06/10/2020</t>
         </is>
       </c>
     </row>
@@ -920,7 +920,7 @@
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>05/04/2021</t>
+          <t>04/05/2021</t>
         </is>
       </c>
     </row>

</xml_diff>